<commit_message>
Heap Implementation containing all the methods of HEAP ADT like percolateUp, percolateDown
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{355AEBCA-CD17-4191-BCF2-328BEB144611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22955F43-1E6B-4151-8B1C-61444FB6904F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="2940" windowWidth="17280" windowHeight="9420" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Problem Desc</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>Heap ADT</t>
+  </si>
+  <si>
+    <t>Problem Link/Details</t>
+  </si>
+  <si>
+    <t>ClassName</t>
+  </si>
+  <si>
+    <t>HeapImpl.java</t>
+  </si>
+  <si>
+    <t>SerialNo</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,12 +407,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merge Sort and updated problems list.
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4DE3D3-78E0-45F8-B377-C36D5D1F955E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254C9421-C5F2-4ED4-83C4-8475F6D716EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Topic</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>InsertionSort</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
+  </si>
+  <si>
+    <t>O(nlogn)</t>
+  </si>
+  <si>
+    <t>O(n)</t>
+  </si>
+  <si>
+    <t>MergeSort ( Stable sorting algo)</t>
   </si>
 </sst>
 </file>
@@ -463,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,6 +599,26 @@
         <v>23</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Selection Problem is implemented.
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B49EF7F-D576-4FA2-807D-B27C9752779F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90549C17-C891-4D06-9DBD-949A52F4CA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Topic</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>QuickSort</t>
+  </si>
+  <si>
+    <t>Selection Algorith</t>
+  </si>
+  <si>
+    <t>Used to find kth position element in sorted array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O(n2) </t>
+  </si>
+  <si>
+    <t>Selection</t>
   </si>
 </sst>
 </file>
@@ -481,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,6 +657,26 @@
         <v>29</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Graph Traversal Algos: Breadth First, Depth First
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB765774-710B-4BCC-851E-BE9FFF120EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEFD689-4068-42EA-8635-CC825B33D333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Topic</t>
   </si>
@@ -140,6 +140,18 @@
   </si>
   <si>
     <t>Adjanceny list impl of graph</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>Depth First Search in Graph</t>
+  </si>
+  <si>
+    <t>Breadth First search in Graph</t>
+  </si>
+  <si>
+    <t>DFS</t>
   </si>
 </sst>
 </file>
@@ -499,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,6 +709,28 @@
         <v>34</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Singly Linked List implementation
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A226B195-7429-4052-A3BE-63B22C72A982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E571593-FFBE-498E-96AC-D1596CEBCA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Topic</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Trie</t>
+  </si>
+  <si>
+    <t>CustomLinkedList</t>
+  </si>
+  <si>
+    <t>Impl of SLL with insert, delete, search, display etc</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,6 +754,20 @@
         <v>41</v>
       </c>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
SLL Loop detection and removal.
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E571593-FFBE-498E-96AC-D1596CEBCA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05420313-737F-4A5C-BA2C-1C04FA0F62C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Topic</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Impl of SLL with insert, delete, search, display etc</t>
+  </si>
+  <si>
+    <t>Detect Loop and Remove Loop</t>
+  </si>
+  <si>
+    <t>RemoveLoop</t>
   </si>
 </sst>
 </file>
@@ -523,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,6 +774,17 @@
         <v>42</v>
       </c>
     </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Anagrams - Hash related problems.
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05420313-737F-4A5C-BA2C-1C04FA0F62C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9945B0C5-0831-464B-8C11-F1250A96AB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>Topic</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>RemoveLoop</t>
+  </si>
+  <si>
+    <t>Checking for Anagrams - Hash</t>
+  </si>
+  <si>
+    <t>CheckAnagrams</t>
+  </si>
+  <si>
+    <t>Hash related problems</t>
   </si>
 </sst>
 </file>
@@ -529,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,6 +794,20 @@
         <v>45</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Hash Bit Set impl
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9945B0C5-0831-464B-8C11-F1250A96AB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1512B4E8-EB8C-4691-A404-DEF34D26A9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Topic</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>Hash related problems</t>
+  </si>
+  <si>
+    <t>Check for first repeated character</t>
+  </si>
+  <si>
+    <t>Hash - BitSet</t>
+  </si>
+  <si>
+    <t>CheckFirstDuplicateUsingBitSet</t>
   </si>
 </sst>
 </file>
@@ -538,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,6 +817,20 @@
         <v>47</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Super Queue using Deque
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E07C30D-574C-4AF0-B165-9D3209E40ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2052A3E5-3BC0-42C9-9A92-EF662C731DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>Topic</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>SuperStack</t>
+  </si>
+  <si>
+    <t>Super Queue</t>
+  </si>
+  <si>
+    <t>SuperQueue</t>
   </si>
 </sst>
 </file>
@@ -571,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,6 +900,20 @@
         <v>58</v>
       </c>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Trees: Complete, BFS Traversal, Threaded Binary tree impl
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2052A3E5-3BC0-42C9-9A92-EF662C731DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDECCC8-217F-409A-8B13-9CD3FC80D3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Topic</t>
   </si>
@@ -218,6 +218,24 @@
   </si>
   <si>
     <t>SuperQueue</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Complete binary tree impl</t>
+  </si>
+  <si>
+    <t>Breadth First search</t>
+  </si>
+  <si>
+    <t>BFS in tree</t>
+  </si>
+  <si>
+    <t>Threaded BT : Inorder traversal and conversion to Threaded BT</t>
+  </si>
+  <si>
+    <t>ThreadedBT</t>
   </si>
 </sst>
 </file>
@@ -577,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,6 +932,45 @@
         <v>61</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tree: Diameter , Morris traversal
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDECCC8-217F-409A-8B13-9CD3FC80D3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34B253F-C770-4FAF-9DEC-29B3D93FCE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Topic</t>
   </si>
@@ -236,6 +237,12 @@
   </si>
   <si>
     <t>ThreadedBT</t>
+  </si>
+  <si>
+    <t>Diameter of binary tree</t>
+  </si>
+  <si>
+    <t>DiameterOfBT</t>
   </si>
 </sst>
 </file>
@@ -595,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,6 +978,17 @@
         <v>67</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Binary Search Tree ADT: insert, delete, search, checking for BST property
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FBF22C-5DCA-41F1-AC24-82C90B770B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8EEB93-A709-41B8-BA90-07B9141479EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
   <si>
     <t>Topic</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>BoundaryOfBT</t>
+  </si>
+  <si>
+    <t>BST all operations</t>
+  </si>
+  <si>
+    <t>BinarySearchTree</t>
   </si>
 </sst>
 </file>
@@ -620,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1040,6 +1046,17 @@
         <v>75</v>
       </c>
     </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Array Problems: Interesting ones
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8EEB93-A709-41B8-BA90-07B9141479EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88002195-8608-42BE-8F65-4086A125DB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10A86EBD-2933-469A-9087-8A02B7160FF7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>Topic</t>
   </si>
@@ -267,6 +267,18 @@
   </si>
   <si>
     <t>BinarySearchTree</t>
+  </si>
+  <si>
+    <t>Longest Band in array</t>
+  </si>
+  <si>
+    <t>LongestBand</t>
+  </si>
+  <si>
+    <t>Smallest Sub arary to sort in array</t>
+  </si>
+  <si>
+    <t>SmallestSubArrayToSort</t>
   </si>
 </sst>
 </file>
@@ -626,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE995BB3-FC62-41CD-BCB1-0A258C74D3CB}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,6 +1069,34 @@
         <v>77</v>
       </c>
     </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BST : Inorder successor
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC46C03-7621-469E-9763-F2DB22199C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7D5271-B857-40B1-87DE-149E5DE36083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
   <si>
     <t>Topic</t>
   </si>
@@ -319,6 +319,12 @@
   </si>
   <si>
     <t>com.nelluri.bsts</t>
+  </si>
+  <si>
+    <t>Find Inorder successor in a BST</t>
+  </si>
+  <si>
+    <t>FindInorderSuccessor</t>
   </si>
 </sst>
 </file>
@@ -681,7 +687,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1242,6 +1248,12 @@
       <c r="A39">
         <v>42</v>
       </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="H39" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Replace with sum at each node.
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7D5271-B857-40B1-87DE-149E5DE36083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B2610-6E8C-4CF2-9D2D-0C3D78599C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="102">
   <si>
     <t>Topic</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>FindInorderSuccessor</t>
+  </si>
+  <si>
+    <t>Replace with Sum</t>
+  </si>
+  <si>
+    <t>ReplaceWithSum</t>
   </si>
 </sst>
 </file>
@@ -684,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,6 +1261,17 @@
         <v>99</v>
       </c>
     </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+      <c r="H40" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Max subset sum, Nodes at Distance K : binary tree problems.
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B2610-6E8C-4CF2-9D2D-0C3D78599C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AE1304-A5AF-4D2D-8525-7FD2D650E371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="106">
   <si>
     <t>Topic</t>
   </si>
@@ -331,13 +331,25 @@
   </si>
   <si>
     <t>ReplaceWithSum</t>
+  </si>
+  <si>
+    <t>Max subset sum tree</t>
+  </si>
+  <si>
+    <t>MaxSubsetSumTree</t>
+  </si>
+  <si>
+    <t>NodesAtDistanceK for binary tree</t>
+  </si>
+  <si>
+    <t>NodesAtDistanceK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +361,12 @@
       <sz val="9.8000000000000007"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -371,9 +389,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -690,13 +711,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.77734375" bestFit="1" customWidth="1"/>
@@ -706,7 +727,7 @@
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -732,7 +753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -749,7 +770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -766,7 +787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -780,7 +801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15.6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -794,7 +815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -814,7 +835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
@@ -834,7 +855,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
@@ -854,7 +875,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
@@ -874,7 +895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
@@ -888,7 +909,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -899,7 +920,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
@@ -910,7 +931,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
@@ -921,7 +942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
@@ -935,7 +956,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
@@ -946,7 +967,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>
@@ -960,7 +981,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>16</v>
       </c>
@@ -974,7 +995,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>17</v>
       </c>
@@ -988,7 +1009,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1002,7 +1023,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1013,7 +1034,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1027,7 +1048,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1041,7 +1062,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1055,7 +1076,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1066,7 +1087,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1077,7 +1098,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1088,7 +1109,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>30</v>
       </c>
@@ -1099,7 +1120,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>31</v>
       </c>
@@ -1110,7 +1131,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>32</v>
       </c>
@@ -1121,7 +1142,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>33</v>
       </c>
@@ -1135,7 +1156,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>34</v>
       </c>
@@ -1149,7 +1170,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>35</v>
       </c>
@@ -1163,7 +1184,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>36</v>
       </c>
@@ -1180,7 +1201,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>37</v>
       </c>
@@ -1197,7 +1218,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>38</v>
       </c>
@@ -1211,7 +1232,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>39</v>
       </c>
@@ -1222,7 +1243,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>40</v>
       </c>
@@ -1233,7 +1254,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>41</v>
       </c>
@@ -1250,7 +1271,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>42</v>
       </c>
@@ -1261,7 +1282,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>43</v>
       </c>
@@ -1270,6 +1291,28 @@
       </c>
       <c r="H40" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="H41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>104</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Max XOR problem using binary trie.
</commit_message>
<xml_diff>
--- a/ProblemsSolved.xlsx
+++ b/ProblemsSolved.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan.Priyanka\IdeaProjects\lc_1000_problems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nelluri\IdeaProjects\lc_1000_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9174507E-7913-48FE-B3E1-8C8657830623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="116">
   <si>
     <t>Topic</t>
   </si>
@@ -361,12 +360,24 @@
   </si>
   <si>
     <t>RotatedSearch</t>
+  </si>
+  <si>
+    <t>Cute little cat</t>
+  </si>
+  <si>
+    <t>CuteCatImpl</t>
+  </si>
+  <si>
+    <t>BiggestXOR problem</t>
+  </si>
+  <si>
+    <t>BiggestXOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -719,11 +730,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,6 +1366,31 @@
         <v>111</v>
       </c>
     </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+      <c r="H46" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>